<commit_message>
Modify not to register empty row
</commit_message>
<xml_diff>
--- a/java/data/dummy_data.xlsx
+++ b/java/data/dummy_data.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\takuya\Dropbox (MIT)\MIT\Claases\2017Fall\1.125 Architecting &amp; Engineering Software Systems\project\balance\java\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\takuya\Dropbox (MIT)\MIT\Claases\2017Fall\1.125 Architecting &amp; Engineering Software Systems\project\balance\java\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8100"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8100" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="task" sheetId="1" r:id="rId1"/>
@@ -25,11 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
-  <si>
-    <t>id</t>
-    <phoneticPr fontId="1"/>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
   <si>
     <t>userId</t>
     <phoneticPr fontId="1"/>
@@ -79,10 +75,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>id</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>studyHour</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -119,7 +111,7 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>xs</t>
+    <t>_id</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -456,10 +448,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -474,46 +466,46 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
-        <v>12</v>
-      </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" t="s">
-        <v>11</v>
-      </c>
       <c r="N1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.4">
@@ -527,7 +519,7 @@
         <v>1.125</v>
       </c>
       <c r="D2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E2">
         <v>5</v>
@@ -539,7 +531,7 @@
         <v>43070</v>
       </c>
       <c r="I2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="J2">
         <v>3</v>
@@ -554,7 +546,7 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="N2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.4">
@@ -568,7 +560,7 @@
         <v>1.125</v>
       </c>
       <c r="D3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E3">
         <v>3</v>
@@ -580,7 +572,7 @@
         <v>43074</v>
       </c>
       <c r="I3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="J3">
         <v>3</v>
@@ -595,12 +587,7 @@
         <v>0.54166666666666663</v>
       </c>
       <c r="N3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="M4" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -614,8 +601,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -627,16 +614,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
         <v>13</v>
-      </c>
-      <c r="B1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.4">
@@ -644,7 +631,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C2">
         <v>8</v>

</xml_diff>

<commit_message>
Change subjectId's format as a text
</commit_message>
<xml_diff>
--- a/java/data/dummy_data.xlsx
+++ b/java/data/dummy_data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8100" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8100"/>
   </bookViews>
   <sheets>
     <sheet name="task" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
   <si>
     <t>userId</t>
     <phoneticPr fontId="1"/>
@@ -112,6 +112,14 @@
   </si>
   <si>
     <t>_id</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>1.125</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>1.125</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -158,7 +166,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -166,6 +174,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -450,8 +461,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -515,8 +526,8 @@
       <c r="B2">
         <v>1</v>
       </c>
-      <c r="C2">
-        <v>1.125</v>
+      <c r="C2" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="D2" t="s">
         <v>17</v>
@@ -556,8 +567,8 @@
       <c r="B3">
         <v>1</v>
       </c>
-      <c r="C3">
-        <v>1.125</v>
+      <c r="C3" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="D3" t="s">
         <v>20</v>
@@ -601,8 +612,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>

</xml_diff>

<commit_message>
Change format of dates
</commit_message>
<xml_diff>
--- a/java/data/dummy_data.xlsx
+++ b/java/data/dummy_data.xlsx
@@ -1,23 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28908"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\takuya\Dropbox (MIT)\MIT\Claases\2017Fall\1.125 Architecting &amp; Engineering Software Systems\project\balance\java\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/takuya/Dropbox (MIT)/MIT/Claases/2017Fall/1.125 Architecting &amp; Engineering Software Systems/project/balance/java/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8100"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="24080" windowHeight="13220"/>
   </bookViews>
   <sheets>
     <sheet name="task" sheetId="1" r:id="rId1"/>
     <sheet name="user" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -47,10 +53,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>dueDate</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>description</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -121,24 +123,31 @@
   <si>
     <t>1.125</t>
     <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>dueDateTime</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="2">
+    <numFmt numFmtId="165" formatCode="m/d/yy\ h:mm;@"/>
+    <numFmt numFmtId="166" formatCode="m/d/yy;@"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="游ゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="6"/>
-      <name val="游ゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -166,17 +175,20 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -459,25 +471,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:N16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="O21" sqref="O21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="6" max="6" width="11.25" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.25" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.83203125" customWidth="1"/>
+    <col min="8" max="8" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.25" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -495,42 +507,42 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>9</v>
       </c>
-      <c r="M1" t="s">
-        <v>10</v>
-      </c>
       <c r="N1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>22</v>
+      <c r="C2" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="D2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E2">
         <v>5</v>
@@ -538,40 +550,40 @@
       <c r="F2">
         <v>5</v>
       </c>
-      <c r="G2" s="1">
-        <v>43070</v>
+      <c r="G2" s="3">
+        <v>43070.999305555553</v>
       </c>
       <c r="I2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J2">
         <v>3</v>
       </c>
-      <c r="K2" s="1">
+      <c r="K2" s="4">
         <v>43070</v>
       </c>
-      <c r="L2" s="2">
+      <c r="L2" s="1">
         <v>0.54166666666666663</v>
       </c>
-      <c r="M2" s="2">
+      <c r="M2" s="1">
         <v>0.66666666666666663</v>
       </c>
       <c r="N2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.4">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>23</v>
+      <c r="C3" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="D3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E3">
         <v>3</v>
@@ -579,27 +591,72 @@
       <c r="F3">
         <v>5</v>
       </c>
-      <c r="G3" s="1">
-        <v>43074</v>
+      <c r="G3" s="3">
+        <v>43074.999305555553</v>
       </c>
       <c r="I3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J3">
         <v>3</v>
       </c>
-      <c r="K3" s="1">
+      <c r="K3" s="4">
         <v>43073</v>
       </c>
-      <c r="L3" s="2">
+      <c r="L3" s="1">
         <v>0.41666666666666669</v>
       </c>
-      <c r="M3" s="2">
+      <c r="M3" s="1">
         <v>0.54166666666666663</v>
       </c>
       <c r="N3" t="s">
-        <v>19</v>
-      </c>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="G4" s="3"/>
+      <c r="K4" s="4"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="G5" s="3"/>
+      <c r="K5" s="4"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="G6" s="3"/>
+      <c r="K6" s="4"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="G7" s="3"/>
+      <c r="K7" s="4"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="G8" s="3"/>
+      <c r="K8" s="4"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="G9" s="3"/>
+      <c r="K9" s="4"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="K10" s="4"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="K11" s="4"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="K12" s="4"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="K13" s="4"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="K14" s="4"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="K15" s="4"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="K16" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
@@ -616,33 +673,33 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="16.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
         <v>12</v>
       </c>
-      <c r="D1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C2">
         <v>8</v>

</xml_diff>